<commit_message>
Nye elektrificeringsgrader fra 2050
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Scen_IND_MIDROAD_Maxshare_constraint.xlsx
+++ b/TIMES-DE/SuppXLS/Scen_IND_MIDROAD_Maxshare_constraint.xlsx
@@ -138,9 +138,6 @@
     <t>UC_FLO~2020</t>
   </si>
   <si>
-    <t>UC_FLO~2060</t>
-  </si>
-  <si>
     <t>UC_RHSRTS~UP~2020</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>IND*</t>
+  </si>
+  <si>
+    <t>UC_FLO~2050</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,13 +596,13 @@
         <v>39</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>10</v>
@@ -625,7 +625,7 @@
         <v>INDSDPH*</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" t="str">
         <f>G6</f>
@@ -696,7 +696,7 @@
         <v>INDCDPH*</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -767,7 +767,7 @@
         <v>INDADPH*</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -838,7 +838,7 @@
         <v>INDGDPH*</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -909,7 +909,7 @@
         <v>INDTDPH*</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -980,7 +980,7 @@
         <v>INDMDPH*</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -1051,7 +1051,7 @@
         <v>INDIDPH*</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -1122,7 +1122,7 @@
         <v>INDFDPH*</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -1193,7 +1193,7 @@
         <v>INDRDPH*</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -1264,7 +1264,7 @@
         <v>INDWDPH*</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -1335,7 +1335,7 @@
         <v>INDLDPH*</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -1406,7 +1406,7 @@
         <v>INDNDPH*</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -1477,7 +1477,7 @@
         <v>INDODPH*</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>

</xml_diff>